<commit_message>
Updated reference designators on Asset_Cal_Info tab from *GL001 to *GL486
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS05MOAS-GL486_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS05MOAS-GL486_00001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="4740" yWindow="3900" windowWidth="25540" windowHeight="11400" tabRatio="377"/>
@@ -90,18 +90,6 @@
     <t>No calibration coefficient</t>
   </si>
   <si>
-    <t>GS05MOAS-GL001-02-DOSTAM000</t>
-  </si>
-  <si>
-    <t>GS05MOAS-GL001-01-FLORDM000</t>
-  </si>
-  <si>
-    <t>GS05MOAS-GL001-04-CTDGVM000</t>
-  </si>
-  <si>
-    <t>GS05MOAS-GL001-00-ENG000000</t>
-  </si>
-  <si>
     <t>CC_scattering_angle</t>
   </si>
   <si>
@@ -148,6 +136,18 @@
   </si>
   <si>
     <t>OL000135</t>
+  </si>
+  <si>
+    <t>GS05MOAS-GL486-01-FLORDM000</t>
+  </si>
+  <si>
+    <t>GS05MOAS-GL486-02-DOSTAM000</t>
+  </si>
+  <si>
+    <t>GS05MOAS-GL486-04-CTDGVM000</t>
+  </si>
+  <si>
+    <t>GS05MOAS-GL486-00-ENG000000</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="42">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>0</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="15">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5">
         <v>486</v>
@@ -800,16 +800,16 @@
         <v>42358</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5">
         <v>1000</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="10">
@@ -845,7 +845,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>14</v>
@@ -875,7 +875,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>10</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>486</v>
@@ -901,27 +901,27 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2">
         <v>3551</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2">
         <v>140</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
         <v>486</v>
@@ -930,27 +930,27 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2">
         <v>3551</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2">
         <v>700</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
         <v>486</v>
@@ -959,27 +959,27 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2">
         <v>3551</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H4" s="11">
         <v>1.0960000000000001</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>486</v>
@@ -988,19 +988,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2">
         <v>3551</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2">
         <v>3.9E-2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1">
@@ -1014,10 +1014,10 @@
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1">
       <c r="A7" s="8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8">
         <v>486</v>
@@ -1026,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F7" s="8">
         <v>323</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8">
         <v>486</v>
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="8">
         <v>9174</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="8">
         <v>486</v>
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8">
         <v>486</v>

</xml_diff>